<commit_message>
update grid location + add new patterns
</commit_message>
<xml_diff>
--- a/game.xlsx
+++ b/game.xlsx
@@ -29,12 +29,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60,9 +69,8 @@
       <font>
         <color theme="0"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -92,20 +100,6 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -383,170 +377,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX50"/>
+  <dimension ref="A1:AY51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+      <selection activeCell="AP31" sqref="AP31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1">
-        <v>0</v>
-      </c>
-      <c r="N1">
-        <v>0</v>
-      </c>
-      <c r="O1">
-        <v>0</v>
-      </c>
-      <c r="P1">
-        <v>0</v>
-      </c>
-      <c r="Q1">
-        <v>0</v>
-      </c>
-      <c r="R1">
-        <v>0</v>
-      </c>
-      <c r="S1">
-        <v>0</v>
-      </c>
-      <c r="T1">
-        <v>0</v>
-      </c>
-      <c r="U1">
-        <v>0</v>
-      </c>
-      <c r="V1">
-        <v>0</v>
-      </c>
-      <c r="W1">
-        <v>0</v>
-      </c>
-      <c r="X1">
-        <v>0</v>
-      </c>
-      <c r="Y1">
-        <v>0</v>
-      </c>
-      <c r="Z1">
-        <v>0</v>
-      </c>
-      <c r="AA1">
-        <v>0</v>
-      </c>
-      <c r="AB1">
-        <v>0</v>
-      </c>
-      <c r="AC1">
-        <v>0</v>
-      </c>
-      <c r="AD1">
-        <v>0</v>
-      </c>
-      <c r="AE1">
-        <v>0</v>
-      </c>
-      <c r="AF1">
-        <v>0</v>
-      </c>
-      <c r="AG1">
-        <v>0</v>
-      </c>
-      <c r="AH1">
-        <v>0</v>
-      </c>
-      <c r="AI1">
-        <v>0</v>
-      </c>
-      <c r="AJ1">
-        <v>0</v>
-      </c>
-      <c r="AK1">
-        <v>0</v>
-      </c>
-      <c r="AL1">
-        <v>0</v>
-      </c>
-      <c r="AM1">
-        <v>0</v>
-      </c>
-      <c r="AN1">
-        <v>0</v>
-      </c>
-      <c r="AO1">
-        <v>0</v>
-      </c>
-      <c r="AP1">
-        <v>0</v>
-      </c>
-      <c r="AQ1">
-        <v>0</v>
-      </c>
-      <c r="AR1">
-        <v>0</v>
-      </c>
-      <c r="AS1">
-        <v>0</v>
-      </c>
-      <c r="AT1">
-        <v>0</v>
-      </c>
-      <c r="AU1">
-        <v>0</v>
-      </c>
-      <c r="AV1">
-        <v>0</v>
-      </c>
-      <c r="AW1">
-        <v>0</v>
-      </c>
-      <c r="AX1">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
       <c r="B2">
         <v>0</v>
       </c>
@@ -691,14 +584,15 @@
       <c r="AW2">
         <v>0</v>
       </c>
-      <c r="AX2">
+      <c r="AX2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
       <c r="B3">
         <v>0</v>
       </c>
@@ -843,14 +737,15 @@
       <c r="AW3">
         <v>0</v>
       </c>
-      <c r="AX3">
+      <c r="AX3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
       <c r="B4">
         <v>0</v>
       </c>
@@ -995,14 +890,15 @@
       <c r="AW4">
         <v>0</v>
       </c>
-      <c r="AX4">
+      <c r="AX4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
       <c r="B5">
         <v>0</v>
       </c>
@@ -1147,14 +1043,15 @@
       <c r="AW5">
         <v>0</v>
       </c>
-      <c r="AX5">
+      <c r="AX5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
       <c r="B6">
         <v>0</v>
       </c>
@@ -1299,14 +1196,15 @@
       <c r="AW6">
         <v>0</v>
       </c>
-      <c r="AX6">
+      <c r="AX6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
       <c r="B7">
         <v>0</v>
       </c>
@@ -1451,14 +1349,15 @@
       <c r="AW7">
         <v>0</v>
       </c>
-      <c r="AX7">
+      <c r="AX7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
       <c r="B8">
         <v>0</v>
       </c>
@@ -1603,14 +1502,15 @@
       <c r="AW8">
         <v>0</v>
       </c>
-      <c r="AX8">
+      <c r="AX8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
       <c r="B9">
         <v>0</v>
       </c>
@@ -1755,14 +1655,15 @@
       <c r="AW9">
         <v>0</v>
       </c>
-      <c r="AX9">
+      <c r="AX9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
       <c r="B10">
         <v>0</v>
       </c>
@@ -1907,14 +1808,15 @@
       <c r="AW10">
         <v>0</v>
       </c>
-      <c r="AX10">
+      <c r="AX10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
       <c r="B11">
         <v>0</v>
       </c>
@@ -2059,14 +1961,15 @@
       <c r="AW11">
         <v>0</v>
       </c>
-      <c r="AX11">
+      <c r="AX11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
       <c r="B12">
         <v>0</v>
       </c>
@@ -2211,14 +2114,15 @@
       <c r="AW12">
         <v>0</v>
       </c>
-      <c r="AX12">
+      <c r="AX12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY12" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
-      </c>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
       <c r="B13">
         <v>0</v>
       </c>
@@ -2363,14 +2267,15 @@
       <c r="AW13">
         <v>0</v>
       </c>
-      <c r="AX13">
+      <c r="AX13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY13" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0</v>
-      </c>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
       <c r="B14">
         <v>0</v>
       </c>
@@ -2515,14 +2420,15 @@
       <c r="AW14">
         <v>0</v>
       </c>
-      <c r="AX14">
+      <c r="AX14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY14" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
-      </c>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
       <c r="B15">
         <v>0</v>
       </c>
@@ -2667,14 +2573,15 @@
       <c r="AW15">
         <v>0</v>
       </c>
-      <c r="AX15">
+      <c r="AX15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY15" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0</v>
-      </c>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
       <c r="B16">
         <v>0</v>
       </c>
@@ -2819,14 +2726,15 @@
       <c r="AW16">
         <v>0</v>
       </c>
-      <c r="AX16">
+      <c r="AX16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0</v>
-      </c>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
       <c r="B17">
         <v>0</v>
       </c>
@@ -2971,14 +2879,15 @@
       <c r="AW17">
         <v>0</v>
       </c>
-      <c r="AX17">
+      <c r="AX17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY17" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>0</v>
-      </c>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
       <c r="B18">
         <v>0</v>
       </c>
@@ -3123,14 +3032,15 @@
       <c r="AW18">
         <v>0</v>
       </c>
-      <c r="AX18">
+      <c r="AX18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY18" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0</v>
-      </c>
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
       <c r="B19">
         <v>0</v>
       </c>
@@ -3275,14 +3185,15 @@
       <c r="AW19">
         <v>0</v>
       </c>
-      <c r="AX19">
+      <c r="AX19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY19" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0</v>
-      </c>
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
       <c r="B20">
         <v>0</v>
       </c>
@@ -3427,14 +3338,15 @@
       <c r="AW20">
         <v>0</v>
       </c>
-      <c r="AX20">
+      <c r="AX20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY20" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>0</v>
-      </c>
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
       <c r="B21">
         <v>0</v>
       </c>
@@ -3579,14 +3491,15 @@
       <c r="AW21">
         <v>0</v>
       </c>
-      <c r="AX21">
+      <c r="AX21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY21" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>0</v>
-      </c>
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
       <c r="B22">
         <v>0</v>
       </c>
@@ -3731,14 +3644,15 @@
       <c r="AW22">
         <v>0</v>
       </c>
-      <c r="AX22">
+      <c r="AX22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY22" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0</v>
-      </c>
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
       <c r="B23">
         <v>0</v>
       </c>
@@ -3883,14 +3797,15 @@
       <c r="AW23">
         <v>0</v>
       </c>
-      <c r="AX23">
+      <c r="AX23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY23" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>0</v>
-      </c>
+    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
       <c r="B24">
         <v>0</v>
       </c>
@@ -4035,14 +3950,15 @@
       <c r="AW24">
         <v>0</v>
       </c>
-      <c r="AX24">
+      <c r="AX24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY24" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>0</v>
-      </c>
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
       <c r="B25">
         <v>0</v>
       </c>
@@ -4187,14 +4103,15 @@
       <c r="AW25">
         <v>0</v>
       </c>
-      <c r="AX25">
+      <c r="AX25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY25" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0</v>
-      </c>
+    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
       <c r="B26">
         <v>0</v>
       </c>
@@ -4339,14 +4256,15 @@
       <c r="AW26">
         <v>0</v>
       </c>
-      <c r="AX26">
+      <c r="AX26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY26" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>0</v>
-      </c>
+    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
       <c r="B27">
         <v>0</v>
       </c>
@@ -4491,14 +4409,15 @@
       <c r="AW27">
         <v>0</v>
       </c>
-      <c r="AX27">
+      <c r="AX27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY27" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0</v>
-      </c>
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
       <c r="B28">
         <v>0</v>
       </c>
@@ -4643,14 +4562,15 @@
       <c r="AW28">
         <v>0</v>
       </c>
-      <c r="AX28">
+      <c r="AX28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY28" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>0</v>
-      </c>
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
       <c r="B29">
         <v>0</v>
       </c>
@@ -4795,14 +4715,15 @@
       <c r="AW29">
         <v>0</v>
       </c>
-      <c r="AX29">
+      <c r="AX29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY29" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>0</v>
-      </c>
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
       <c r="B30">
         <v>0</v>
       </c>
@@ -4947,14 +4868,15 @@
       <c r="AW30">
         <v>0</v>
       </c>
-      <c r="AX30">
+      <c r="AX30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY30" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>0</v>
-      </c>
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
       <c r="B31">
         <v>0</v>
       </c>
@@ -5099,14 +5021,15 @@
       <c r="AW31">
         <v>0</v>
       </c>
-      <c r="AX31">
+      <c r="AX31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY31" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0</v>
-      </c>
+    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
       <c r="B32">
         <v>0</v>
       </c>
@@ -5251,14 +5174,15 @@
       <c r="AW32">
         <v>0</v>
       </c>
-      <c r="AX32">
+      <c r="AX32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY32" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>0</v>
-      </c>
+    <row r="33" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
       <c r="B33">
         <v>0</v>
       </c>
@@ -5403,14 +5327,15 @@
       <c r="AW33">
         <v>0</v>
       </c>
-      <c r="AX33">
+      <c r="AX33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY33" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>0</v>
-      </c>
+    <row r="34" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
       <c r="B34">
         <v>0</v>
       </c>
@@ -5555,14 +5480,15 @@
       <c r="AW34">
         <v>0</v>
       </c>
-      <c r="AX34">
+      <c r="AX34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY34" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>0</v>
-      </c>
+    <row r="35" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
       <c r="B35">
         <v>0</v>
       </c>
@@ -5707,14 +5633,15 @@
       <c r="AW35">
         <v>0</v>
       </c>
-      <c r="AX35">
+      <c r="AX35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY35" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>0</v>
-      </c>
+    <row r="36" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
       <c r="B36">
         <v>0</v>
       </c>
@@ -5859,14 +5786,15 @@
       <c r="AW36">
         <v>0</v>
       </c>
-      <c r="AX36">
+      <c r="AX36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY36" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>0</v>
-      </c>
+    <row r="37" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
       <c r="B37">
         <v>0</v>
       </c>
@@ -6011,14 +5939,15 @@
       <c r="AW37">
         <v>0</v>
       </c>
-      <c r="AX37">
+      <c r="AX37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY37" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>0</v>
-      </c>
+    <row r="38" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
       <c r="B38">
         <v>0</v>
       </c>
@@ -6163,14 +6092,15 @@
       <c r="AW38">
         <v>0</v>
       </c>
-      <c r="AX38">
+      <c r="AX38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY38" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>0</v>
-      </c>
+    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
       <c r="B39">
         <v>0</v>
       </c>
@@ -6315,14 +6245,15 @@
       <c r="AW39">
         <v>0</v>
       </c>
-      <c r="AX39">
+      <c r="AX39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY39" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>0</v>
-      </c>
+    <row r="40" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
       <c r="B40">
         <v>0</v>
       </c>
@@ -6467,14 +6398,15 @@
       <c r="AW40">
         <v>0</v>
       </c>
-      <c r="AX40">
+      <c r="AX40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY40" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>0</v>
-      </c>
+    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
       <c r="B41">
         <v>0</v>
       </c>
@@ -6619,14 +6551,15 @@
       <c r="AW41">
         <v>0</v>
       </c>
-      <c r="AX41">
+      <c r="AX41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY41" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>0</v>
-      </c>
+    <row r="42" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
       <c r="B42">
         <v>0</v>
       </c>
@@ -6771,14 +6704,15 @@
       <c r="AW42">
         <v>0</v>
       </c>
-      <c r="AX42">
+      <c r="AX42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY42" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>0</v>
-      </c>
+    <row r="43" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
       <c r="B43">
         <v>0</v>
       </c>
@@ -6923,14 +6857,15 @@
       <c r="AW43">
         <v>0</v>
       </c>
-      <c r="AX43">
+      <c r="AX43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY43" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>0</v>
-      </c>
+    <row r="44" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
       <c r="B44">
         <v>0</v>
       </c>
@@ -7075,14 +7010,15 @@
       <c r="AW44">
         <v>0</v>
       </c>
-      <c r="AX44">
+      <c r="AX44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY44" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>0</v>
-      </c>
+    <row r="45" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
       <c r="B45">
         <v>0</v>
       </c>
@@ -7227,14 +7163,15 @@
       <c r="AW45">
         <v>0</v>
       </c>
-      <c r="AX45">
+      <c r="AX45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY45" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>0</v>
-      </c>
+    <row r="46" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
       <c r="B46">
         <v>0</v>
       </c>
@@ -7379,14 +7316,15 @@
       <c r="AW46">
         <v>0</v>
       </c>
-      <c r="AX46">
+      <c r="AX46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY46" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>0</v>
-      </c>
+    <row r="47" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
       <c r="B47">
         <v>0</v>
       </c>
@@ -7531,14 +7469,15 @@
       <c r="AW47">
         <v>0</v>
       </c>
-      <c r="AX47">
+      <c r="AX47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY47" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>0</v>
-      </c>
+    <row r="48" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
       <c r="B48">
         <v>0</v>
       </c>
@@ -7683,14 +7622,15 @@
       <c r="AW48">
         <v>0</v>
       </c>
-      <c r="AX48">
+      <c r="AX48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY48" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>0</v>
-      </c>
+    <row r="49" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
       <c r="B49">
         <v>0</v>
       </c>
@@ -7835,14 +7775,15 @@
       <c r="AW49">
         <v>0</v>
       </c>
-      <c r="AX49">
+      <c r="AX49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY49" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>0</v>
-      </c>
+    <row r="50" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
       <c r="B50">
         <v>0</v>
       </c>
@@ -7987,17 +7928,75 @@
       <c r="AW50">
         <v>0</v>
       </c>
-      <c r="AX50">
+      <c r="AX50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="3"/>
+      <c r="AC51" s="3"/>
+      <c r="AD51" s="3"/>
+      <c r="AE51" s="3"/>
+      <c r="AF51" s="3"/>
+      <c r="AG51" s="3"/>
+      <c r="AH51" s="3"/>
+      <c r="AI51" s="3"/>
+      <c r="AJ51" s="3"/>
+      <c r="AK51" s="3"/>
+      <c r="AL51" s="3"/>
+      <c r="AM51" s="3"/>
+      <c r="AN51" s="3"/>
+      <c r="AO51" s="3"/>
+      <c r="AP51" s="3"/>
+      <c r="AQ51" s="3"/>
+      <c r="AR51" s="3"/>
+      <c r="AS51" s="3"/>
+      <c r="AT51" s="3"/>
+      <c r="AU51" s="3"/>
+      <c r="AV51" s="3"/>
+      <c r="AW51" s="3"/>
+      <c r="AX51" s="3"/>
+      <c r="AY51" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="B2:AX50">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added forced ui creation + more patterns
</commit_message>
<xml_diff>
--- a/game.xlsx
+++ b/game.xlsx
@@ -442,15 +442,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CY54"/>
+  <dimension ref="A1:DB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB26" sqref="AB26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -554,8 +552,11 @@
       <c r="CW1" s="1"/>
       <c r="CX1" s="1"/>
       <c r="CY1" s="1"/>
+      <c r="CZ1" s="1"/>
+      <c r="DA1" s="1"/>
+      <c r="DB1" s="1"/>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="1">
         <v>0</v>
@@ -759,8 +760,11 @@
       <c r="CW2" s="1"/>
       <c r="CX2" s="1"/>
       <c r="CY2" s="1"/>
+      <c r="CZ2" s="1"/>
+      <c r="DA2" s="1"/>
+      <c r="DB2" s="1"/>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="1">
         <v>0</v>
@@ -964,8 +968,11 @@
       <c r="CW3" s="1"/>
       <c r="CX3" s="1"/>
       <c r="CY3" s="1"/>
+      <c r="CZ3" s="1"/>
+      <c r="DA3" s="1"/>
+      <c r="DB3" s="1"/>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="1">
         <v>0</v>
@@ -1169,8 +1176,11 @@
       <c r="CW4" s="1"/>
       <c r="CX4" s="1"/>
       <c r="CY4" s="1"/>
+      <c r="CZ4" s="1"/>
+      <c r="DA4" s="1"/>
+      <c r="DB4" s="1"/>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="1">
         <v>0</v>
@@ -1374,8 +1384,11 @@
       <c r="CW5" s="1"/>
       <c r="CX5" s="1"/>
       <c r="CY5" s="1"/>
+      <c r="CZ5" s="1"/>
+      <c r="DA5" s="1"/>
+      <c r="DB5" s="1"/>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="1">
         <v>0</v>
@@ -1579,8 +1592,11 @@
       <c r="CW6" s="1"/>
       <c r="CX6" s="1"/>
       <c r="CY6" s="1"/>
+      <c r="CZ6" s="1"/>
+      <c r="DA6" s="1"/>
+      <c r="DB6" s="1"/>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="1">
         <v>0</v>
@@ -1784,8 +1800,11 @@
       <c r="CW7" s="1"/>
       <c r="CX7" s="1"/>
       <c r="CY7" s="1"/>
+      <c r="CZ7" s="1"/>
+      <c r="DA7" s="1"/>
+      <c r="DB7" s="1"/>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="1">
         <v>0</v>
@@ -1989,8 +2008,11 @@
       <c r="CW8" s="1"/>
       <c r="CX8" s="1"/>
       <c r="CY8" s="1"/>
+      <c r="CZ8" s="1"/>
+      <c r="DA8" s="1"/>
+      <c r="DB8" s="1"/>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="1">
         <v>0</v>
@@ -2194,8 +2216,11 @@
       <c r="CW9" s="1"/>
       <c r="CX9" s="1"/>
       <c r="CY9" s="1"/>
+      <c r="CZ9" s="1"/>
+      <c r="DA9" s="1"/>
+      <c r="DB9" s="1"/>
     </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="1">
         <v>0</v>
@@ -2399,8 +2424,11 @@
       <c r="CW10" s="1"/>
       <c r="CX10" s="1"/>
       <c r="CY10" s="1"/>
+      <c r="CZ10" s="1"/>
+      <c r="DA10" s="1"/>
+      <c r="DB10" s="1"/>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="1">
         <v>0</v>
@@ -2604,8 +2632,11 @@
       <c r="CW11" s="1"/>
       <c r="CX11" s="1"/>
       <c r="CY11" s="1"/>
+      <c r="CZ11" s="1"/>
+      <c r="DA11" s="1"/>
+      <c r="DB11" s="1"/>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="1">
         <v>0</v>
@@ -2809,8 +2840,11 @@
       <c r="CW12" s="1"/>
       <c r="CX12" s="1"/>
       <c r="CY12" s="1"/>
+      <c r="CZ12" s="1"/>
+      <c r="DA12" s="1"/>
+      <c r="DB12" s="1"/>
     </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="1">
         <v>0</v>
@@ -3014,8 +3048,11 @@
       <c r="CW13" s="1"/>
       <c r="CX13" s="1"/>
       <c r="CY13" s="1"/>
+      <c r="CZ13" s="1"/>
+      <c r="DA13" s="1"/>
+      <c r="DB13" s="1"/>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="1">
         <v>0</v>
@@ -3219,8 +3256,11 @@
       <c r="CW14" s="1"/>
       <c r="CX14" s="1"/>
       <c r="CY14" s="1"/>
+      <c r="CZ14" s="1"/>
+      <c r="DA14" s="1"/>
+      <c r="DB14" s="1"/>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="1">
         <v>0</v>
@@ -3424,8 +3464,11 @@
       <c r="CW15" s="1"/>
       <c r="CX15" s="1"/>
       <c r="CY15" s="1"/>
+      <c r="CZ15" s="1"/>
+      <c r="DA15" s="1"/>
+      <c r="DB15" s="1"/>
     </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="1">
         <v>0</v>
@@ -3629,8 +3672,11 @@
       <c r="CW16" s="1"/>
       <c r="CX16" s="1"/>
       <c r="CY16" s="1"/>
+      <c r="CZ16" s="1"/>
+      <c r="DA16" s="1"/>
+      <c r="DB16" s="1"/>
     </row>
-    <row r="17" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="1">
         <v>0</v>
@@ -3834,8 +3880,11 @@
       <c r="CW17" s="1"/>
       <c r="CX17" s="1"/>
       <c r="CY17" s="1"/>
+      <c r="CZ17" s="1"/>
+      <c r="DA17" s="1"/>
+      <c r="DB17" s="1"/>
     </row>
-    <row r="18" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="1">
         <v>0</v>
@@ -4039,8 +4088,11 @@
       <c r="CW18" s="1"/>
       <c r="CX18" s="1"/>
       <c r="CY18" s="1"/>
+      <c r="CZ18" s="1"/>
+      <c r="DA18" s="1"/>
+      <c r="DB18" s="1"/>
     </row>
-    <row r="19" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="1">
         <v>0</v>
@@ -4244,8 +4296,11 @@
       <c r="CW19" s="1"/>
       <c r="CX19" s="1"/>
       <c r="CY19" s="1"/>
+      <c r="CZ19" s="1"/>
+      <c r="DA19" s="1"/>
+      <c r="DB19" s="1"/>
     </row>
-    <row r="20" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="1">
         <v>0</v>
@@ -4449,8 +4504,11 @@
       <c r="CW20" s="1"/>
       <c r="CX20" s="1"/>
       <c r="CY20" s="1"/>
+      <c r="CZ20" s="1"/>
+      <c r="DA20" s="1"/>
+      <c r="DB20" s="1"/>
     </row>
-    <row r="21" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="1">
         <v>0</v>
@@ -4654,8 +4712,11 @@
       <c r="CW21" s="1"/>
       <c r="CX21" s="1"/>
       <c r="CY21" s="1"/>
+      <c r="CZ21" s="1"/>
+      <c r="DA21" s="1"/>
+      <c r="DB21" s="1"/>
     </row>
-    <row r="22" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="1">
         <v>0</v>
@@ -4859,8 +4920,11 @@
       <c r="CW22" s="1"/>
       <c r="CX22" s="1"/>
       <c r="CY22" s="1"/>
+      <c r="CZ22" s="1"/>
+      <c r="DA22" s="1"/>
+      <c r="DB22" s="1"/>
     </row>
-    <row r="23" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="1">
         <v>0</v>
@@ -5064,8 +5128,11 @@
       <c r="CW23" s="1"/>
       <c r="CX23" s="1"/>
       <c r="CY23" s="1"/>
+      <c r="CZ23" s="1"/>
+      <c r="DA23" s="1"/>
+      <c r="DB23" s="1"/>
     </row>
-    <row r="24" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="1">
         <v>0</v>
@@ -5269,8 +5336,11 @@
       <c r="CW24" s="1"/>
       <c r="CX24" s="1"/>
       <c r="CY24" s="1"/>
+      <c r="CZ24" s="1"/>
+      <c r="DA24" s="1"/>
+      <c r="DB24" s="1"/>
     </row>
-    <row r="25" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="1">
         <v>0</v>
@@ -5474,8 +5544,11 @@
       <c r="CW25" s="1"/>
       <c r="CX25" s="1"/>
       <c r="CY25" s="1"/>
+      <c r="CZ25" s="1"/>
+      <c r="DA25" s="1"/>
+      <c r="DB25" s="1"/>
     </row>
-    <row r="26" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="1">
         <v>0</v>
@@ -5679,8 +5752,11 @@
       <c r="CW26" s="1"/>
       <c r="CX26" s="1"/>
       <c r="CY26" s="1"/>
+      <c r="CZ26" s="1"/>
+      <c r="DA26" s="1"/>
+      <c r="DB26" s="1"/>
     </row>
-    <row r="27" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="1">
         <v>0</v>
@@ -5884,8 +5960,11 @@
       <c r="CW27" s="1"/>
       <c r="CX27" s="1"/>
       <c r="CY27" s="1"/>
+      <c r="CZ27" s="1"/>
+      <c r="DA27" s="1"/>
+      <c r="DB27" s="1"/>
     </row>
-    <row r="28" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="1">
         <v>0</v>
@@ -6089,8 +6168,11 @@
       <c r="CW28" s="1"/>
       <c r="CX28" s="1"/>
       <c r="CY28" s="1"/>
+      <c r="CZ28" s="1"/>
+      <c r="DA28" s="1"/>
+      <c r="DB28" s="1"/>
     </row>
-    <row r="29" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="1">
         <v>0</v>
@@ -6294,8 +6376,11 @@
       <c r="CW29" s="1"/>
       <c r="CX29" s="1"/>
       <c r="CY29" s="1"/>
+      <c r="CZ29" s="1"/>
+      <c r="DA29" s="1"/>
+      <c r="DB29" s="1"/>
     </row>
-    <row r="30" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="1">
         <v>0</v>
@@ -6499,8 +6584,11 @@
       <c r="CW30" s="1"/>
       <c r="CX30" s="1"/>
       <c r="CY30" s="1"/>
+      <c r="CZ30" s="1"/>
+      <c r="DA30" s="1"/>
+      <c r="DB30" s="1"/>
     </row>
-    <row r="31" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="1">
         <v>0</v>
@@ -6704,8 +6792,11 @@
       <c r="CW31" s="1"/>
       <c r="CX31" s="1"/>
       <c r="CY31" s="1"/>
+      <c r="CZ31" s="1"/>
+      <c r="DA31" s="1"/>
+      <c r="DB31" s="1"/>
     </row>
-    <row r="32" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="1">
         <v>0</v>
@@ -6909,8 +7000,11 @@
       <c r="CW32" s="1"/>
       <c r="CX32" s="1"/>
       <c r="CY32" s="1"/>
+      <c r="CZ32" s="1"/>
+      <c r="DA32" s="1"/>
+      <c r="DB32" s="1"/>
     </row>
-    <row r="33" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="1">
         <v>0</v>
@@ -7114,8 +7208,11 @@
       <c r="CW33" s="1"/>
       <c r="CX33" s="1"/>
       <c r="CY33" s="1"/>
+      <c r="CZ33" s="1"/>
+      <c r="DA33" s="1"/>
+      <c r="DB33" s="1"/>
     </row>
-    <row r="34" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="1">
         <v>0</v>
@@ -7319,8 +7416,11 @@
       <c r="CW34" s="1"/>
       <c r="CX34" s="1"/>
       <c r="CY34" s="1"/>
+      <c r="CZ34" s="1"/>
+      <c r="DA34" s="1"/>
+      <c r="DB34" s="1"/>
     </row>
-    <row r="35" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="1">
         <v>0</v>
@@ -7524,8 +7624,11 @@
       <c r="CW35" s="1"/>
       <c r="CX35" s="1"/>
       <c r="CY35" s="1"/>
+      <c r="CZ35" s="1"/>
+      <c r="DA35" s="1"/>
+      <c r="DB35" s="1"/>
     </row>
-    <row r="36" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="1">
         <v>0</v>
@@ -7729,8 +7832,11 @@
       <c r="CW36" s="1"/>
       <c r="CX36" s="1"/>
       <c r="CY36" s="1"/>
+      <c r="CZ36" s="1"/>
+      <c r="DA36" s="1"/>
+      <c r="DB36" s="1"/>
     </row>
-    <row r="37" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="1">
         <v>0</v>
@@ -7934,8 +8040,11 @@
       <c r="CW37" s="1"/>
       <c r="CX37" s="1"/>
       <c r="CY37" s="1"/>
+      <c r="CZ37" s="1"/>
+      <c r="DA37" s="1"/>
+      <c r="DB37" s="1"/>
     </row>
-    <row r="38" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="1">
         <v>0</v>
@@ -8139,8 +8248,11 @@
       <c r="CW38" s="1"/>
       <c r="CX38" s="1"/>
       <c r="CY38" s="1"/>
+      <c r="CZ38" s="1"/>
+      <c r="DA38" s="1"/>
+      <c r="DB38" s="1"/>
     </row>
-    <row r="39" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="1">
         <v>0</v>
@@ -8344,8 +8456,11 @@
       <c r="CW39" s="1"/>
       <c r="CX39" s="1"/>
       <c r="CY39" s="1"/>
+      <c r="CZ39" s="1"/>
+      <c r="DA39" s="1"/>
+      <c r="DB39" s="1"/>
     </row>
-    <row r="40" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="1">
         <v>0</v>
@@ -8549,8 +8664,11 @@
       <c r="CW40" s="1"/>
       <c r="CX40" s="1"/>
       <c r="CY40" s="1"/>
+      <c r="CZ40" s="1"/>
+      <c r="DA40" s="1"/>
+      <c r="DB40" s="1"/>
     </row>
-    <row r="41" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="1">
         <v>0</v>
@@ -8754,8 +8872,11 @@
       <c r="CW41" s="1"/>
       <c r="CX41" s="1"/>
       <c r="CY41" s="1"/>
+      <c r="CZ41" s="1"/>
+      <c r="DA41" s="1"/>
+      <c r="DB41" s="1"/>
     </row>
-    <row r="42" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="1">
         <v>0</v>
@@ -8959,8 +9080,11 @@
       <c r="CW42" s="1"/>
       <c r="CX42" s="1"/>
       <c r="CY42" s="1"/>
+      <c r="CZ42" s="1"/>
+      <c r="DA42" s="1"/>
+      <c r="DB42" s="1"/>
     </row>
-    <row r="43" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="1">
         <v>0</v>
@@ -9164,8 +9288,11 @@
       <c r="CW43" s="1"/>
       <c r="CX43" s="1"/>
       <c r="CY43" s="1"/>
+      <c r="CZ43" s="1"/>
+      <c r="DA43" s="1"/>
+      <c r="DB43" s="1"/>
     </row>
-    <row r="44" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="1">
         <v>0</v>
@@ -9369,8 +9496,11 @@
       <c r="CW44" s="1"/>
       <c r="CX44" s="1"/>
       <c r="CY44" s="1"/>
+      <c r="CZ44" s="1"/>
+      <c r="DA44" s="1"/>
+      <c r="DB44" s="1"/>
     </row>
-    <row r="45" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="1">
         <v>0</v>
@@ -9574,8 +9704,11 @@
       <c r="CW45" s="1"/>
       <c r="CX45" s="1"/>
       <c r="CY45" s="1"/>
+      <c r="CZ45" s="1"/>
+      <c r="DA45" s="1"/>
+      <c r="DB45" s="1"/>
     </row>
-    <row r="46" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="1">
         <v>0</v>
@@ -9778,8 +9911,12 @@
       <c r="CV46" s="1"/>
       <c r="CW46" s="1"/>
       <c r="CX46" s="1"/>
+      <c r="CY46" s="1"/>
+      <c r="CZ46" s="1"/>
+      <c r="DA46" s="1"/>
+      <c r="DB46" s="1"/>
     </row>
-    <row r="47" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="1">
         <v>0</v>
@@ -9987,8 +10124,13 @@
       <c r="CU47" s="10"/>
       <c r="CV47" s="1"/>
       <c r="CW47" s="1"/>
+      <c r="CX47" s="1"/>
+      <c r="CY47" s="1"/>
+      <c r="CZ47" s="1"/>
+      <c r="DA47" s="1"/>
+      <c r="DB47" s="1"/>
     </row>
-    <row r="48" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="1">
         <v>0</v>
@@ -10190,8 +10332,13 @@
       <c r="CU48" s="10"/>
       <c r="CV48" s="1"/>
       <c r="CW48" s="1"/>
+      <c r="CX48" s="1"/>
+      <c r="CY48" s="1"/>
+      <c r="CZ48" s="1"/>
+      <c r="DA48" s="1"/>
+      <c r="DB48" s="1"/>
     </row>
-    <row r="49" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="1">
         <v>0</v>
@@ -10393,8 +10540,13 @@
       <c r="CU49" s="10"/>
       <c r="CV49" s="1"/>
       <c r="CW49" s="1"/>
+      <c r="CX49" s="1"/>
+      <c r="CY49" s="1"/>
+      <c r="CZ49" s="1"/>
+      <c r="DA49" s="1"/>
+      <c r="DB49" s="1"/>
     </row>
-    <row r="50" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="1">
         <v>0</v>
@@ -10596,8 +10748,13 @@
       <c r="CU50" s="10"/>
       <c r="CV50" s="1"/>
       <c r="CW50" s="1"/>
+      <c r="CX50" s="1"/>
+      <c r="CY50" s="1"/>
+      <c r="CZ50" s="1"/>
+      <c r="DA50" s="1"/>
+      <c r="DB50" s="1"/>
     </row>
-    <row r="51" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="1">
         <v>0</v>
@@ -10799,8 +10956,13 @@
       <c r="CU51" s="10"/>
       <c r="CV51" s="1"/>
       <c r="CW51" s="1"/>
+      <c r="CX51" s="1"/>
+      <c r="CY51" s="1"/>
+      <c r="CZ51" s="1"/>
+      <c r="DA51" s="1"/>
+      <c r="DB51" s="1"/>
     </row>
-    <row r="52" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -10902,8 +11064,13 @@
       <c r="CU52" s="10"/>
       <c r="CV52" s="1"/>
       <c r="CW52" s="1"/>
+      <c r="CX52" s="1"/>
+      <c r="CY52" s="1"/>
+      <c r="CZ52" s="1"/>
+      <c r="DA52" s="1"/>
+      <c r="DB52" s="1"/>
     </row>
-    <row r="53" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -11006,7 +11173,7 @@
       <c r="CV53" s="1"/>
       <c r="CW53" s="1"/>
     </row>
-    <row r="54" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="BB47:BT52"/>

</xml_diff>